<commit_message>
price added to dataset
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F62"/>
+  <dimension ref="A1:G62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -464,6 +464,11 @@
           <t>tip</t>
         </is>
       </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>fiyat</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -496,6 +501,11 @@
           <t>bot</t>
         </is>
       </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2799 </t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -528,6 +538,11 @@
           <t>bot</t>
         </is>
       </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2799 </t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -560,6 +575,11 @@
           <t>bot</t>
         </is>
       </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2799 </t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -592,6 +612,11 @@
           <t>bot</t>
         </is>
       </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2799 </t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -624,6 +649,11 @@
           <t>bot</t>
         </is>
       </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2799 </t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -656,6 +686,11 @@
           <t>bot</t>
         </is>
       </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2799 </t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -688,6 +723,11 @@
           <t>bot</t>
         </is>
       </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">3699 </t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -720,6 +760,11 @@
           <t>bot</t>
         </is>
       </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2799 </t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -752,6 +797,11 @@
           <t>bot</t>
         </is>
       </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">3699 </t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -782,6 +832,11 @@
       <c r="F11" t="inlineStr">
         <is>
           <t>bot</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">3699 </t>
         </is>
       </c>
     </row>
@@ -808,6 +863,11 @@
           <t>bot</t>
         </is>
       </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">3699 </t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -832,6 +892,11 @@
           <t>bot</t>
         </is>
       </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">3699 </t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -856,6 +921,11 @@
           <t>bot</t>
         </is>
       </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2799 </t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -880,6 +950,11 @@
           <t>bot</t>
         </is>
       </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">3699 </t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -912,6 +987,11 @@
           <t>bot</t>
         </is>
       </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2799 </t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -942,6 +1022,11 @@
       <c r="F17" t="inlineStr">
         <is>
           <t>bot</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2799 </t>
         </is>
       </c>
     </row>
@@ -968,6 +1053,11 @@
           <t>bot</t>
         </is>
       </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2799 </t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -992,6 +1082,11 @@
           <t>bot</t>
         </is>
       </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2799 </t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1020,6 +1115,11 @@
           <t>bot</t>
         </is>
       </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2799 </t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1048,6 +1148,11 @@
           <t>bot</t>
         </is>
       </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2799 </t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1076,6 +1181,11 @@
           <t>ayakkabı</t>
         </is>
       </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t xml:space="preserve">263912 </t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1104,6 +1214,11 @@
           <t>ayakkabı</t>
         </is>
       </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t xml:space="preserve">263912 </t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1136,6 +1251,11 @@
           <t>ayakkabı</t>
         </is>
       </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t xml:space="preserve">3499 </t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1168,6 +1288,11 @@
           <t>ayakkabı</t>
         </is>
       </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t xml:space="preserve">3499 </t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1200,6 +1325,11 @@
           <t>bot</t>
         </is>
       </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2499 </t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1232,6 +1362,11 @@
           <t>bot</t>
         </is>
       </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2499 </t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1264,6 +1399,11 @@
           <t>ayakkabı</t>
         </is>
       </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1849 </t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1296,6 +1436,11 @@
           <t>ayakkabı</t>
         </is>
       </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1849 </t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1328,6 +1473,11 @@
           <t>ayakkabı</t>
         </is>
       </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2449 </t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1358,6 +1508,11 @@
       <c r="F31" t="inlineStr">
         <is>
           <t>ayakkabı</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2449 </t>
         </is>
       </c>
     </row>
@@ -1376,6 +1531,11 @@
         </is>
       </c>
       <c r="F32" t="inlineStr"/>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2549 </t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1392,6 +1552,11 @@
         </is>
       </c>
       <c r="F33" t="inlineStr"/>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2549 </t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1416,6 +1581,11 @@
         </is>
       </c>
       <c r="F34" t="inlineStr"/>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t xml:space="preserve">3749 </t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1440,6 +1610,11 @@
         </is>
       </c>
       <c r="F35" t="inlineStr"/>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t xml:space="preserve">3749 </t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1468,6 +1643,11 @@
           <t>bot</t>
         </is>
       </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2799 </t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1496,6 +1676,11 @@
           <t>bot</t>
         </is>
       </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2799 </t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1528,6 +1713,11 @@
           <t>bot</t>
         </is>
       </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1699 </t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1560,6 +1750,11 @@
           <t>bot</t>
         </is>
       </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1699 </t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1592,6 +1787,11 @@
           <t>bot</t>
         </is>
       </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1899 </t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1624,6 +1824,11 @@
           <t>bot</t>
         </is>
       </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1699 </t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -1656,6 +1861,11 @@
           <t>bot</t>
         </is>
       </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2999 </t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -1688,110 +1898,184 @@
           <t>bot</t>
         </is>
       </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2999 </t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t xml:space="preserve">Harley Davidson </t>
+          <t xml:space="preserve">F By Fabrika </t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Kauçuk</t>
-        </is>
-      </c>
-      <c r="C44" t="inlineStr"/>
-      <c r="D44" t="inlineStr"/>
+          <t>Termo</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Deri</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>Türkiye</t>
+        </is>
+      </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>kadın</t>
-        </is>
-      </c>
-      <c r="F44" t="inlineStr"/>
+          <t>erkek</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>bot</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t xml:space="preserve">48499 </t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t xml:space="preserve">Harley Davidson </t>
+          <t xml:space="preserve">F By Fabrika </t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Kauçuk</t>
+          <t>Termo</t>
         </is>
       </c>
       <c r="C45" t="inlineStr"/>
-      <c r="D45" t="inlineStr"/>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Türkiye</t>
+        </is>
+      </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>kadın</t>
-        </is>
-      </c>
-      <c r="F45" t="inlineStr"/>
+          <t>erkek</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>bot</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t xml:space="preserve">60999 </t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t xml:space="preserve">Harley Davidson </t>
+          <t xml:space="preserve">F By Fabrika </t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Kauçuk</t>
-        </is>
-      </c>
-      <c r="C46" t="inlineStr"/>
-      <c r="D46" t="inlineStr"/>
+          <t>Termo</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Deri</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>Türkiye</t>
+        </is>
+      </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>kadın</t>
-        </is>
-      </c>
-      <c r="F46" t="inlineStr"/>
+          <t>erkek</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>bot</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t xml:space="preserve">48499 </t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t xml:space="preserve">Harley Davidson </t>
+          <t xml:space="preserve">F By Fabrika </t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Kauçuk</t>
-        </is>
-      </c>
-      <c r="C47" t="inlineStr"/>
-      <c r="D47" t="inlineStr"/>
+          <t>Termo</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Deri</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>Türkiye</t>
+        </is>
+      </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>kadın</t>
+          <t>erkek</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
           <t>bot</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t xml:space="preserve">57499 </t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t xml:space="preserve">Harley Davidson </t>
-        </is>
-      </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>Kauçuk</t>
-        </is>
-      </c>
+          <t xml:space="preserve">F By Fabrika </t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr"/>
       <c r="C48" t="inlineStr"/>
-      <c r="D48" t="inlineStr"/>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Türkiye</t>
+        </is>
+      </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>kadın</t>
-        </is>
-      </c>
-      <c r="F48" t="inlineStr"/>
+          <t>erkek</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>bot</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t xml:space="preserve">50999 </t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -1824,164 +2108,150 @@
           <t>bot</t>
         </is>
       </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t xml:space="preserve">48499 </t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t xml:space="preserve">F By Fabrika </t>
+          <t xml:space="preserve">Harley Davidson </t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Termo</t>
+          <t>Kauçuk</t>
         </is>
       </c>
       <c r="C50" t="inlineStr"/>
-      <c r="D50" t="inlineStr">
-        <is>
-          <t>Türkiye</t>
-        </is>
-      </c>
+      <c r="D50" t="inlineStr"/>
       <c r="E50" t="inlineStr">
         <is>
-          <t>erkek</t>
-        </is>
-      </c>
-      <c r="F50" t="inlineStr">
-        <is>
-          <t>bot</t>
+          <t>kadın</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr"/>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2999 </t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t xml:space="preserve">F By Fabrika </t>
+          <t xml:space="preserve">Harley Davidson </t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Termo</t>
-        </is>
-      </c>
-      <c r="C51" t="inlineStr">
-        <is>
-          <t>Deri</t>
-        </is>
-      </c>
-      <c r="D51" t="inlineStr">
-        <is>
-          <t>Türkiye</t>
-        </is>
-      </c>
+          <t>Kauçuk</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr"/>
+      <c r="D51" t="inlineStr"/>
       <c r="E51" t="inlineStr">
         <is>
-          <t>erkek</t>
-        </is>
-      </c>
-      <c r="F51" t="inlineStr">
-        <is>
-          <t>bot</t>
+          <t>kadın</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr"/>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2999 </t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t xml:space="preserve">F By Fabrika </t>
+          <t xml:space="preserve">Harley Davidson </t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Termo</t>
-        </is>
-      </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>Deri</t>
-        </is>
-      </c>
-      <c r="D52" t="inlineStr">
-        <is>
-          <t>Türkiye</t>
-        </is>
-      </c>
+          <t>Kauçuk</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr"/>
+      <c r="D52" t="inlineStr"/>
       <c r="E52" t="inlineStr">
         <is>
-          <t>erkek</t>
-        </is>
-      </c>
-      <c r="F52" t="inlineStr">
-        <is>
-          <t>bot</t>
+          <t>kadın</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr"/>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2999 </t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t xml:space="preserve">F By Fabrika </t>
-        </is>
-      </c>
-      <c r="B53" t="inlineStr"/>
+          <t xml:space="preserve">Harley Davidson </t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Kauçuk</t>
+        </is>
+      </c>
       <c r="C53" t="inlineStr"/>
-      <c r="D53" t="inlineStr">
-        <is>
-          <t>Türkiye</t>
-        </is>
-      </c>
+      <c r="D53" t="inlineStr"/>
       <c r="E53" t="inlineStr">
         <is>
-          <t>erkek</t>
+          <t>kadın</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
           <t>bot</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t xml:space="preserve">3999 </t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t xml:space="preserve">F By Fabrika </t>
+          <t xml:space="preserve">Harley Davidson </t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Termo</t>
-        </is>
-      </c>
-      <c r="C54" t="inlineStr">
-        <is>
-          <t>Deri</t>
-        </is>
-      </c>
-      <c r="D54" t="inlineStr">
-        <is>
-          <t>Türkiye</t>
-        </is>
-      </c>
+          <t>Kauçuk</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr"/>
+      <c r="D54" t="inlineStr"/>
       <c r="E54" t="inlineStr">
         <is>
-          <t>erkek</t>
-        </is>
-      </c>
-      <c r="F54" t="inlineStr">
-        <is>
-          <t>bot</t>
+          <t>kadın</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr"/>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2999 </t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t xml:space="preserve">Harley Davidson </t>
+          <t xml:space="preserve">Skechers </t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Kauçuk</t>
+          <t>Poliüretan</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -1989,31 +2259,28 @@
           <t>Deri</t>
         </is>
       </c>
-      <c r="D55" t="inlineStr">
-        <is>
-          <t>Türkiye</t>
-        </is>
-      </c>
+      <c r="D55" t="inlineStr"/>
       <c r="E55" t="inlineStr">
         <is>
-          <t>kadın</t>
-        </is>
-      </c>
-      <c r="F55" t="inlineStr">
-        <is>
-          <t>bot</t>
+          <t>erkek</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr"/>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2849 </t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t xml:space="preserve">Harley Davidson </t>
+          <t xml:space="preserve">Skechers </t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Kauçuk</t>
+          <t>Poliüretan</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -2021,31 +2288,28 @@
           <t>Deri</t>
         </is>
       </c>
-      <c r="D56" t="inlineStr">
-        <is>
-          <t>Türkiye</t>
-        </is>
-      </c>
+      <c r="D56" t="inlineStr"/>
       <c r="E56" t="inlineStr">
         <is>
-          <t>kadın</t>
-        </is>
-      </c>
-      <c r="F56" t="inlineStr">
-        <is>
-          <t>bot</t>
+          <t>erkek</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr"/>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2849 </t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t xml:space="preserve">Skechers </t>
+          <t xml:space="preserve">Harley Davidson </t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Poliüretan</t>
+          <t>Kauçuk</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -2053,23 +2317,36 @@
           <t>Deri</t>
         </is>
       </c>
-      <c r="D57" t="inlineStr"/>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>Türkiye</t>
+        </is>
+      </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>erkek</t>
-        </is>
-      </c>
-      <c r="F57" t="inlineStr"/>
+          <t>kadın</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>bot</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t xml:space="preserve">3999 </t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t xml:space="preserve">Skechers </t>
+          <t xml:space="preserve">Harley Davidson </t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Poliüretan</t>
+          <t>Kauçuk</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -2077,117 +2354,150 @@
           <t>Deri</t>
         </is>
       </c>
-      <c r="D58" t="inlineStr"/>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>Türkiye</t>
+        </is>
+      </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>erkek</t>
-        </is>
-      </c>
-      <c r="F58" t="inlineStr"/>
+          <t>kadın</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>bot</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t xml:space="preserve">3999 </t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t xml:space="preserve">Pierre Cardin </t>
+          <t xml:space="preserve">New Balance </t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>EVA</t>
-        </is>
-      </c>
-      <c r="C59" t="inlineStr">
-        <is>
-          <t>Tekstil</t>
-        </is>
-      </c>
-      <c r="D59" t="inlineStr">
-        <is>
-          <t>Türkiye</t>
-        </is>
-      </c>
+          <t>Kauçuk</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr"/>
+      <c r="D59" t="inlineStr"/>
       <c r="E59" t="inlineStr">
         <is>
           <t>kadın</t>
         </is>
       </c>
-      <c r="F59" t="inlineStr">
-        <is>
-          <t>bot</t>
+      <c r="F59" t="inlineStr"/>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1799 </t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t xml:space="preserve">Pierre Cardin </t>
+          <t xml:space="preserve">New Balance </t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>EVA</t>
-        </is>
-      </c>
-      <c r="C60" t="inlineStr">
-        <is>
-          <t>Tekstil</t>
-        </is>
-      </c>
-      <c r="D60" t="inlineStr">
-        <is>
-          <t>Türkiye</t>
-        </is>
-      </c>
+          <t>Kauçuk</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr"/>
+      <c r="D60" t="inlineStr"/>
       <c r="E60" t="inlineStr">
         <is>
           <t>kadın</t>
         </is>
       </c>
-      <c r="F60" t="inlineStr">
-        <is>
-          <t>bot</t>
+      <c r="F60" t="inlineStr"/>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1799 </t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t xml:space="preserve">New Balance </t>
+          <t xml:space="preserve">Pierre Cardin </t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Kauçuk</t>
-        </is>
-      </c>
-      <c r="C61" t="inlineStr"/>
-      <c r="D61" t="inlineStr"/>
+          <t>EVA</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Tekstil</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>Türkiye</t>
+        </is>
+      </c>
       <c r="E61" t="inlineStr">
         <is>
           <t>kadın</t>
         </is>
       </c>
-      <c r="F61" t="inlineStr"/>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>bot</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t xml:space="preserve">89990 </t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t xml:space="preserve">New Balance </t>
+          <t xml:space="preserve">Pierre Cardin </t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Kauçuk</t>
-        </is>
-      </c>
-      <c r="C62" t="inlineStr"/>
-      <c r="D62" t="inlineStr"/>
+          <t>EVA</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Tekstil</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>Türkiye</t>
+        </is>
+      </c>
       <c r="E62" t="inlineStr">
         <is>
           <t>kadın</t>
         </is>
       </c>
-      <c r="F62" t="inlineStr"/>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>bot</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t xml:space="preserve">89990 </t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
save the mL models
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -4897,7 +4897,9 @@
       <c r="D138" t="inlineStr"/>
       <c r="E138" t="inlineStr"/>
       <c r="F138" t="inlineStr"/>
-      <c r="G138" t="inlineStr"/>
+      <c r="G138" t="n">
+        <v>2699</v>
+      </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">

</xml_diff>